<commit_message>
rebuilding the stats table in english
</commit_message>
<xml_diff>
--- a/projects/en/docs/assets/tables/GDMBR.xlsx
+++ b/projects/en/docs/assets/tables/GDMBR.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gravel/Private/f3/docs/assets/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gravel/Private/f3/projects/en/docs/assets/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20831FA8-07F9-C14F-8BA3-5A6618626728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CB49CF-F115-4243-81A2-9AA160783D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="680" windowWidth="25560" windowHeight="20400" xr2:uid="{3D076BE0-CA79-3448-855F-AD0FA0DCE9D7}"/>
+    <workbookView xWindow="660" yWindow="680" windowWidth="38260" windowHeight="23520" xr2:uid="{3D076BE0-CA79-3448-855F-AD0FA0DCE9D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="299">
   <si>
     <t>When</t>
   </si>
@@ -1294,127 +1295,136 @@
     <t>day43</t>
   </si>
   <si>
-    <t>Sunset Post</t>
-  </si>
-  <si>
-    <t>Camaraderie</t>
-  </si>
-  <si>
-    <t>Pie Town and Toaster House</t>
-  </si>
-  <si>
-    <t>Deserticus</t>
-  </si>
-  <si>
-    <t>Abiquiu to Cuba</t>
-  </si>
-  <si>
-    <t>Abiquiu Lodge</t>
-  </si>
-  <si>
-    <t>Land of enchantement - really?</t>
-  </si>
-  <si>
-    <t>Altus Maximus</t>
-  </si>
-  <si>
-    <t>Del Norte - le Colorado sauvage</t>
-  </si>
-  <si>
-    <t>Cow-Girl</t>
-  </si>
-  <si>
-    <t>Salida et un peu de repos</t>
-  </si>
-  <si>
-    <t>Boreas Pass 3'500m</t>
-  </si>
-  <si>
-    <t>le Colorado a du relief!</t>
-  </si>
-  <si>
-    <t>Leaving Brush Mountain Lodge</t>
-  </si>
-  <si>
-    <t>Hello Colorado!</t>
-  </si>
-  <si>
-    <t>Ça déraille à Rawlins</t>
-  </si>
-  <si>
-    <t>The Great Basin #2</t>
-  </si>
-  <si>
-    <t>The Great Basin</t>
-  </si>
-  <si>
-    <t>Pinendale</t>
-  </si>
-  <si>
-    <t>Togwotee et Union Pass</t>
-  </si>
-  <si>
-    <t>Welcome in Wyoming</t>
-  </si>
-  <si>
-    <t>Old Oregon Short Line</t>
-  </si>
-  <si>
-    <t>Today is a good day</t>
-  </si>
-  <si>
-    <t>Orages</t>
-  </si>
-  <si>
-    <t>Fleecer Ridge</t>
-  </si>
-  <si>
-    <t>2 semaines</t>
-  </si>
-  <si>
-    <t>Lava Mountain and Butte</t>
-  </si>
-  <si>
-    <t>Helena et Park Lake</t>
-  </si>
-  <si>
-    <t>1'000km</t>
-  </si>
-  <si>
-    <t>Alpaca Farm</t>
-  </si>
-  <si>
-    <t>2075mD+</t>
-  </si>
-  <si>
-    <t>Camping chez Swan!</t>
-  </si>
-  <si>
-    <t>une semaine déjà!</t>
-  </si>
-  <si>
-    <t>49ème parallèle</t>
-  </si>
-  <si>
-    <t>the Titan</t>
-  </si>
-  <si>
-    <t>the King</t>
-  </si>
-  <si>
-    <t>Le jour du Grand Départ</t>
-  </si>
-  <si>
-    <t>Arrivée à Banff</t>
-  </si>
-  <si>
-    <t>On fait pas le malin le 1er jour</t>
-  </si>
-  <si>
-    <t>Antelope Wells : clap de fin. Vraiment ?</t>
-  </si>
-  <si>
     <t>From BANFF = 40 days</t>
+  </si>
+  <si>
+    <t>43. Sunset Post</t>
+  </si>
+  <si>
+    <t>42. Antelope Wells: the final stretch 💪. Really?</t>
+  </si>
+  <si>
+    <t>41. Hachita</t>
+  </si>
+  <si>
+    <t>39. Camaraderie</t>
+  </si>
+  <si>
+    <t>39. Beaverhead Ranch</t>
+  </si>
+  <si>
+    <t>38. Pie Town and Toaster House</t>
+  </si>
+  <si>
+    <t>37. Grants</t>
+  </si>
+  <si>
+    <t>36. Deserticus</t>
+  </si>
+  <si>
+    <t>35. Abiquiu to Cuba</t>
+  </si>
+  <si>
+    <t>34. Abiquiu Lodge</t>
+  </si>
+  <si>
+    <t>33. Land of Enchantment - Really?</t>
+  </si>
+  <si>
+    <t>32. Altus Maximus</t>
+  </si>
+  <si>
+    <t>31. Del Norte - The Wild Colorado</t>
+  </si>
+  <si>
+    <t>30. Cow-Girl encounter</t>
+  </si>
+  <si>
+    <t>29. Salida and a Bit of Rest</t>
+  </si>
+  <si>
+    <t>28. Boreas Pass 3,500 m</t>
+  </si>
+  <si>
+    <t>27. Colorado Has Relief!</t>
+  </si>
+  <si>
+    <t>26. Leaving Brush Mountain Lodge</t>
+  </si>
+  <si>
+    <t>25. Hello Colorado!</t>
+  </si>
+  <si>
+    <t>24. Things Go Wrong in Rawlins</t>
+  </si>
+  <si>
+    <t>23. The Great Basin #2</t>
+  </si>
+  <si>
+    <t>22. The Great Basin</t>
+  </si>
+  <si>
+    <t>21. Pinendale</t>
+  </si>
+  <si>
+    <t>20. Togwotee and Union Pass</t>
+  </si>
+  <si>
+    <t>19. Welcome to Wyoming</t>
+  </si>
+  <si>
+    <t>18. Old Oregon Short Line</t>
+  </si>
+  <si>
+    <t>17. Today is a Good Day</t>
+  </si>
+  <si>
+    <t>16. Storms</t>
+  </si>
+  <si>
+    <t>15. Fleecer Ridge</t>
+  </si>
+  <si>
+    <t>14. It's been 2 Weeks</t>
+  </si>
+  <si>
+    <t>13. Lava Mountain and Butte</t>
+  </si>
+  <si>
+    <t>12. Helena and Park Lake</t>
+  </si>
+  <si>
+    <t>11. The 1,000 km mark</t>
+  </si>
+  <si>
+    <t>10. The Alpaca Farm</t>
+  </si>
+  <si>
+    <t>9. Overcoming 2075mD+</t>
+  </si>
+  <si>
+    <t>8. Camping at Swan!</t>
+  </si>
+  <si>
+    <t>7. A week already!</t>
+  </si>
+  <si>
+    <t>6. The 49th Parallel</t>
+  </si>
+  <si>
+    <t>5. The Titan</t>
+  </si>
+  <si>
+    <t>4. The King</t>
+  </si>
+  <si>
+    <t>3. The Day of the Grand Depart</t>
+  </si>
+  <si>
+    <t>2. Arrival in Banff</t>
+  </si>
+  <si>
+    <t>1. Not Showing Off on the First Day</t>
   </si>
 </sst>
 </file>
@@ -1877,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB97B946-75B5-864A-A3A5-6F8B2DC55CE3}">
   <dimension ref="A1:AI55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1889,7 +1899,7 @@
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" customWidth="1"/>
     <col min="6" max="6" width="8.1640625" customWidth="1"/>
-    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47.83203125" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" customWidth="1"/>
     <col min="10" max="10" width="86" customWidth="1"/>
@@ -2038,7 +2048,7 @@
         <v>254</v>
       </c>
       <c r="G2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>149</v>
@@ -2146,7 +2156,7 @@
         <v>253</v>
       </c>
       <c r="G3" t="s">
-        <v>294</v>
+        <v>257</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>148</v>
@@ -2254,7 +2264,7 @@
         <v>251</v>
       </c>
       <c r="G4" t="s">
-        <v>148</v>
+        <v>258</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>150</v>
@@ -2362,7 +2372,7 @@
         <v>252</v>
       </c>
       <c r="G5" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>152</v>
@@ -2470,7 +2480,7 @@
         <v>214</v>
       </c>
       <c r="G6" t="s">
-        <v>152</v>
+        <v>260</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>151</v>
@@ -2578,7 +2588,7 @@
         <v>215</v>
       </c>
       <c r="G7" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>154</v>
@@ -2686,7 +2696,7 @@
         <v>216</v>
       </c>
       <c r="G8" t="s">
-        <v>154</v>
+        <v>262</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>155</v>
@@ -2794,7 +2804,7 @@
         <v>217</v>
       </c>
       <c r="G9" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>153</v>
@@ -2902,7 +2912,7 @@
         <v>218</v>
       </c>
       <c r="G10" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>156</v>
@@ -3010,7 +3020,7 @@
         <v>219</v>
       </c>
       <c r="G11" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -3116,7 +3126,7 @@
         <v>220</v>
       </c>
       <c r="G12" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="1" t="s">
@@ -3221,7 +3231,7 @@
         <v>221</v>
       </c>
       <c r="G13" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>157</v>
@@ -3329,7 +3339,7 @@
         <v>222</v>
       </c>
       <c r="G14" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>160</v>
@@ -3437,7 +3447,7 @@
         <v>223</v>
       </c>
       <c r="G15" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -3543,7 +3553,7 @@
         <v>224</v>
       </c>
       <c r="G16" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>158</v>
@@ -3651,7 +3661,7 @@
         <v>225</v>
       </c>
       <c r="G17" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>159</v>
@@ -3759,7 +3769,7 @@
         <v>226</v>
       </c>
       <c r="G18" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -3865,7 +3875,7 @@
         <v>227</v>
       </c>
       <c r="G19" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -3971,7 +3981,7 @@
         <v>228</v>
       </c>
       <c r="G20" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -4077,7 +4087,7 @@
         <v>229</v>
       </c>
       <c r="G21" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -4183,7 +4193,7 @@
         <v>230</v>
       </c>
       <c r="G22" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -4289,7 +4299,7 @@
         <v>231</v>
       </c>
       <c r="G23" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -4395,7 +4405,7 @@
         <v>232</v>
       </c>
       <c r="G24" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -4501,7 +4511,7 @@
         <v>233</v>
       </c>
       <c r="G25" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -4607,7 +4617,7 @@
         <v>234</v>
       </c>
       <c r="G26" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -4713,7 +4723,7 @@
         <v>235</v>
       </c>
       <c r="G27" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -4819,7 +4829,7 @@
         <v>236</v>
       </c>
       <c r="G28" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -4925,7 +4935,7 @@
         <v>237</v>
       </c>
       <c r="G29" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -5031,7 +5041,7 @@
         <v>238</v>
       </c>
       <c r="G30" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -5137,7 +5147,7 @@
         <v>239</v>
       </c>
       <c r="G31" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -5243,7 +5253,7 @@
         <v>240</v>
       </c>
       <c r="G32" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>140</v>
@@ -5350,7 +5360,7 @@
         <v>241</v>
       </c>
       <c r="G33" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>210</v>
@@ -5453,7 +5463,7 @@
         <v>242</v>
       </c>
       <c r="G34" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>139</v>
@@ -5515,7 +5525,7 @@
         <v>243</v>
       </c>
       <c r="G35" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>139</v>
@@ -5623,7 +5633,7 @@
         <v>244</v>
       </c>
       <c r="G36" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -5729,7 +5739,7 @@
         <v>245</v>
       </c>
       <c r="G37" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -5835,7 +5845,7 @@
         <v>246</v>
       </c>
       <c r="G38" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>132</v>
@@ -5945,7 +5955,7 @@
         <v>247</v>
       </c>
       <c r="G39" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>131</v>
@@ -6055,7 +6065,7 @@
         <v>248</v>
       </c>
       <c r="G40" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>130</v>
@@ -6165,7 +6175,7 @@
         <v>249</v>
       </c>
       <c r="G41" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>129</v>
@@ -6275,7 +6285,7 @@
         <v>250</v>
       </c>
       <c r="G42" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>128</v>
@@ -6385,7 +6395,7 @@
         <v>213</v>
       </c>
       <c r="G43" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>145</v>
@@ -6494,7 +6504,7 @@
         <v>212</v>
       </c>
       <c r="G44" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>127</v>
@@ -6642,7 +6652,7 @@
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="1" t="s">
-        <v>295</v>
+        <v>255</v>
       </c>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
cleaning up french version
</commit_message>
<xml_diff>
--- a/projects/en/docs/assets/tables/GDMBR.xlsx
+++ b/projects/en/docs/assets/tables/GDMBR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gravel/Private/f3/projects/en/docs/assets/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CB49CF-F115-4243-81A2-9AA160783D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EDB82C-215F-B649-B6CD-A6EA29C863C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="680" windowWidth="38260" windowHeight="23520" xr2:uid="{3D076BE0-CA79-3448-855F-AD0FA0DCE9D7}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="14900" windowWidth="25600" windowHeight="13900" xr2:uid="{3D076BE0-CA79-3448-855F-AD0FA0DCE9D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="277">
   <si>
     <t>When</t>
   </si>
@@ -917,18 +917,6 @@
     <t>Banff, Grand Depart, Spray Lake</t>
   </si>
   <si>
-    <t>Spray Lake, Elkford</t>
-  </si>
-  <si>
-    <t>Elkford, Fernie</t>
-  </si>
-  <si>
-    <t>Fernie, US Border, Eureka</t>
-  </si>
-  <si>
-    <t>Eureka, Bicycle Station, Red Meadow Lake, Whitefish</t>
-  </si>
-  <si>
     <t>BUTTS CABIN?</t>
   </si>
   <si>
@@ -950,9 +938,6 @@
     <t>Lama Ranch</t>
   </si>
   <si>
-    <t>Butte</t>
-  </si>
-  <si>
     <t>DAYS &gt;&gt;</t>
   </si>
   <si>
@@ -1019,135 +1004,6 @@
     <t>Day</t>
   </si>
   <si>
-    <t>Zero Day</t>
-  </si>
-  <si>
-    <t>Day 42</t>
-  </si>
-  <si>
-    <t>Day 41</t>
-  </si>
-  <si>
-    <t>Day 40</t>
-  </si>
-  <si>
-    <t>Day 39</t>
-  </si>
-  <si>
-    <t>Day 38</t>
-  </si>
-  <si>
-    <t>Day 37</t>
-  </si>
-  <si>
-    <t>Day 36</t>
-  </si>
-  <si>
-    <t>Day 35</t>
-  </si>
-  <si>
-    <t>Day 34</t>
-  </si>
-  <si>
-    <t>Day 33</t>
-  </si>
-  <si>
-    <t>Day 32</t>
-  </si>
-  <si>
-    <t>Day 31</t>
-  </si>
-  <si>
-    <t>Day 30</t>
-  </si>
-  <si>
-    <t>Day 29</t>
-  </si>
-  <si>
-    <t>Day 28</t>
-  </si>
-  <si>
-    <t>Day 27</t>
-  </si>
-  <si>
-    <t>Day 26</t>
-  </si>
-  <si>
-    <t>Day 25</t>
-  </si>
-  <si>
-    <t>Day 24</t>
-  </si>
-  <si>
-    <t>Day 23</t>
-  </si>
-  <si>
-    <t>Day 22</t>
-  </si>
-  <si>
-    <t>Day 21</t>
-  </si>
-  <si>
-    <t>Day 20</t>
-  </si>
-  <si>
-    <t>Day 19</t>
-  </si>
-  <si>
-    <t>Day 18</t>
-  </si>
-  <si>
-    <t>Day 17</t>
-  </si>
-  <si>
-    <t>Day 16</t>
-  </si>
-  <si>
-    <t>Day 15</t>
-  </si>
-  <si>
-    <t>Day 14</t>
-  </si>
-  <si>
-    <t>Day 13</t>
-  </si>
-  <si>
-    <t>Day 12</t>
-  </si>
-  <si>
-    <t>Day 11</t>
-  </si>
-  <si>
-    <t>Day 10</t>
-  </si>
-  <si>
-    <t>Day 9</t>
-  </si>
-  <si>
-    <t>Day 8</t>
-  </si>
-  <si>
-    <t>Day 7</t>
-  </si>
-  <si>
-    <t>Day 6</t>
-  </si>
-  <si>
-    <t>Day 5</t>
-  </si>
-  <si>
-    <t>Day 4</t>
-  </si>
-  <si>
-    <t>Day 3</t>
-  </si>
-  <si>
-    <t>Day 2</t>
-  </si>
-  <si>
-    <t>Day 1</t>
-  </si>
-  <si>
     <t>remove after</t>
   </si>
   <si>
@@ -1160,9 +1016,6 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>Helena</t>
-  </si>
-  <si>
     <t>Blog title</t>
   </si>
   <si>
@@ -1425,6 +1278,87 @@
   </si>
   <si>
     <t>1. Not Showing Off on the First Day</t>
+  </si>
+  <si>
+    <t>Strava mapping does not work after Lama Ranch</t>
+  </si>
+  <si>
+    <t>Sunset Post (San Diego) - there should be no strava link?</t>
+  </si>
+  <si>
+    <t>Day 15 is also misrepresented</t>
+  </si>
+  <si>
+    <t>Fernie, US Border, Eureka, Bicycle Station</t>
+  </si>
+  <si>
+    <t>Bicycle Station, Red Meadow Lake, Whitefish</t>
+  </si>
+  <si>
+    <t>Spray Lake, Grizzly, Elkford</t>
+  </si>
+  <si>
+    <t>Elkford, Sparwood &amp; Titan, Fernie, John&amp;John</t>
+  </si>
+  <si>
+    <t>Columbia Falls, Swan River</t>
+  </si>
+  <si>
+    <t>Clearwater Lake, Single Trail, Seeley Lake (missed)</t>
+  </si>
+  <si>
+    <t>Helena, Park Lake for me alone</t>
+  </si>
+  <si>
+    <t>Day 12 vs Day 11 need to be inverted (based on gpx)</t>
+  </si>
+  <si>
+    <t>Lava Mountain, Basin (Burger then Siesta), Butte</t>
+  </si>
+  <si>
+    <t>Thompson Park, The Other Sarah #1, Fleecer Ridge starts</t>
+  </si>
+  <si>
+    <t>Fleecer Ridge Continues, Wiseriver (Pizza, Cougar), Elkhorn Hot Springs</t>
+  </si>
+  <si>
+    <t>Ma Barnes, Banack Road, Stormy Night</t>
+  </si>
+  <si>
+    <t>Cabesone Canyon, Big Sheep River, Lima (Highway station)</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Red Rock Lakes  Refuge, Old Railroad, Warm River Campground, Smore</t>
+  </si>
+  <si>
+    <t>Rainy climb, Jackson Lake, Colton Bay, Grand Teton Park</t>
+  </si>
+  <si>
+    <t>Robert Cabin &amp; Shower, Togwotee and Union Pass</t>
+  </si>
+  <si>
+    <t>Union Pass long downhill and Pinendale</t>
+  </si>
+  <si>
+    <t>South Pass City, Atlantic City, Diagnus Well</t>
+  </si>
+  <si>
+    <t>Headwind, Invisible Hand, Rawlins</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Aspen Valley, Brush Mountain Lodge</t>
+  </si>
+  <si>
+    <t>Derailleur Cable Fix</t>
   </si>
 </sst>
 </file>
@@ -1522,7 +1456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1550,6 +1484,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1888,7 +1823,7 @@
   <dimension ref="A1:AI55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1897,10 +1832,10 @@
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="8.1640625" customWidth="1"/>
     <col min="7" max="7" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.83203125" customWidth="1"/>
+    <col min="8" max="8" width="59.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" customWidth="1"/>
     <col min="10" max="10" width="86" customWidth="1"/>
     <col min="13" max="13" width="11.6640625" customWidth="1"/>
@@ -1921,34 +1856,34 @@
   <sheetData>
     <row r="1" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>208</v>
+        <v>160</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>125</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>206</v>
+        <v>158</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>211</v>
+        <v>162</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>126</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="K1" s="15" t="s">
         <v>92</v>
@@ -2020,15 +1955,16 @@
         <v>110</v>
       </c>
       <c r="AH1" s="14" t="s">
-        <v>207</v>
+        <v>159</v>
       </c>
       <c r="AI1" s="17" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>164</v>
+      <c r="A2" t="str">
+        <f t="shared" ref="A2:A43" si="0">"Day "&amp;E2</f>
+        <v>Day 43</v>
       </c>
       <c r="B2" s="5">
         <v>45541.271261574075</v>
@@ -2037,21 +1973,20 @@
         <v>121</v>
       </c>
       <c r="D2" s="5" t="str">
-        <f t="shared" ref="D2:D43" si="0">"gpxday"&amp;E2</f>
-        <v>gpxday42</v>
+        <f t="shared" ref="D2:D43" si="1">"gpxday"&amp;E2</f>
+        <v>gpxday43</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E42" si="1">E3+1</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>254</v>
+        <v>205</v>
       </c>
       <c r="G2" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="1" t="s">
@@ -2135,8 +2070,9 @@
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>165</v>
+      <c r="A3" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 42</v>
       </c>
       <c r="B3" s="5">
         <v>45540.331388888888</v>
@@ -2145,21 +2081,20 @@
         <v>122</v>
       </c>
       <c r="D3" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday41</v>
+        <f t="shared" si="1"/>
+        <v>gpxday42</v>
       </c>
       <c r="E3">
-        <f t="shared" si="1"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>253</v>
+        <v>204</v>
       </c>
       <c r="G3" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="1" t="s">
@@ -2243,8 +2178,9 @@
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>166</v>
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 41</v>
       </c>
       <c r="B4" s="5">
         <v>45539.361481481479</v>
@@ -2253,21 +2189,20 @@
         <v>122</v>
       </c>
       <c r="D4" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday40</v>
+        <f t="shared" si="1"/>
+        <v>gpxday41</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>251</v>
+        <v>202</v>
       </c>
       <c r="G4" t="s">
-        <v>258</v>
+        <v>209</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="1" t="s">
@@ -2351,8 +2286,9 @@
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>167</v>
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 40</v>
       </c>
       <c r="B5" s="5">
         <v>45538.317199074074</v>
@@ -2361,21 +2297,20 @@
         <v>122</v>
       </c>
       <c r="D5" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday39</v>
+        <f t="shared" si="1"/>
+        <v>gpxday40</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>252</v>
+        <v>203</v>
       </c>
       <c r="G5" t="s">
-        <v>259</v>
+        <v>210</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="1" t="s">
@@ -2459,8 +2394,9 @@
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>168</v>
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 39</v>
       </c>
       <c r="B6" s="5">
         <v>45537.330150462964</v>
@@ -2469,21 +2405,20 @@
         <v>122</v>
       </c>
       <c r="D6" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday38</v>
+        <f t="shared" si="1"/>
+        <v>gpxday39</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>214</v>
+        <v>165</v>
       </c>
       <c r="G6" t="s">
-        <v>260</v>
+        <v>211</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="1" t="s">
@@ -2567,8 +2502,9 @@
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>169</v>
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 38</v>
       </c>
       <c r="B7" s="5">
         <v>45536.35292824074</v>
@@ -2577,21 +2513,20 @@
         <v>122</v>
       </c>
       <c r="D7" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday37</v>
+        <f t="shared" si="1"/>
+        <v>gpxday38</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>215</v>
+        <v>166</v>
       </c>
       <c r="G7" t="s">
-        <v>261</v>
+        <v>212</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="1" t="s">
@@ -2675,8 +2610,9 @@
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>170</v>
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 37</v>
       </c>
       <c r="B8" s="5">
         <v>45535.437650462962</v>
@@ -2685,21 +2621,20 @@
         <v>122</v>
       </c>
       <c r="D8" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday36</v>
+        <f t="shared" si="1"/>
+        <v>gpxday37</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>216</v>
+        <v>167</v>
       </c>
       <c r="G8" t="s">
-        <v>262</v>
+        <v>213</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="1" t="s">
@@ -2783,8 +2718,9 @@
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>171</v>
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 36</v>
       </c>
       <c r="B9" s="5">
         <v>45534.28628472222</v>
@@ -2793,21 +2729,20 @@
         <v>122</v>
       </c>
       <c r="D9" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday35</v>
+        <f t="shared" si="1"/>
+        <v>gpxday36</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>217</v>
+        <v>168</v>
       </c>
       <c r="G9" t="s">
-        <v>263</v>
+        <v>214</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="1" t="s">
@@ -2891,8 +2826,9 @@
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>172</v>
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 35</v>
       </c>
       <c r="B10" s="5">
         <v>45533.350763888891</v>
@@ -2901,21 +2837,20 @@
         <v>122</v>
       </c>
       <c r="D10" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday34</v>
+        <f t="shared" si="1"/>
+        <v>gpxday35</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>218</v>
+        <v>169</v>
       </c>
       <c r="G10" t="s">
-        <v>264</v>
+        <v>215</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="1" t="s">
@@ -2999,8 +2934,9 @@
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>173</v>
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 34</v>
       </c>
       <c r="B11" s="5">
         <v>45532.418807870374</v>
@@ -3009,18 +2945,17 @@
         <v>122</v>
       </c>
       <c r="D11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday33</v>
+        <f t="shared" si="1"/>
+        <v>gpxday34</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>219</v>
+        <v>170</v>
       </c>
       <c r="G11" t="s">
-        <v>265</v>
+        <v>216</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -3105,8 +3040,9 @@
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>174</v>
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 33</v>
       </c>
       <c r="B12" s="5">
         <v>45531.37226851852</v>
@@ -3115,18 +3051,17 @@
         <v>122</v>
       </c>
       <c r="D12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday32</v>
+        <f t="shared" si="1"/>
+        <v>gpxday33</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>220</v>
+        <v>171</v>
       </c>
       <c r="G12" t="s">
-        <v>266</v>
+        <v>217</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="1" t="s">
@@ -3210,8 +3145,9 @@
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>175</v>
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 32</v>
       </c>
       <c r="B13" s="5">
         <v>45530.375324074077</v>
@@ -3220,21 +3156,20 @@
         <v>122</v>
       </c>
       <c r="D13" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday31</v>
+        <f t="shared" si="1"/>
+        <v>gpxday32</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>221</v>
+        <v>172</v>
       </c>
       <c r="G13" t="s">
-        <v>267</v>
+        <v>218</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="1" t="s">
@@ -3318,8 +3253,9 @@
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>176</v>
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 31</v>
       </c>
       <c r="B14" s="5">
         <v>45529.42564814815</v>
@@ -3328,21 +3264,20 @@
         <v>122</v>
       </c>
       <c r="D14" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday30</v>
+        <f t="shared" si="1"/>
+        <v>gpxday31</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>222</v>
+        <v>173</v>
       </c>
       <c r="G14" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="1" t="s">
@@ -3426,8 +3361,9 @@
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>177</v>
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 30</v>
       </c>
       <c r="B15" s="5">
         <v>45528.701655092591</v>
@@ -3436,18 +3372,17 @@
         <v>121</v>
       </c>
       <c r="D15" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday29</v>
+        <f t="shared" si="1"/>
+        <v>gpxday30</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>223</v>
+        <v>174</v>
       </c>
       <c r="G15" t="s">
-        <v>269</v>
+        <v>220</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -3532,8 +3467,9 @@
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>178</v>
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 29</v>
       </c>
       <c r="B16" s="5">
         <v>45527.323622685188</v>
@@ -3542,21 +3478,20 @@
         <v>122</v>
       </c>
       <c r="D16" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday28</v>
+        <f t="shared" si="1"/>
+        <v>gpxday29</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>224</v>
+        <v>175</v>
       </c>
       <c r="G16" t="s">
-        <v>270</v>
+        <v>221</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="1" t="s">
@@ -3640,8 +3575,9 @@
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>179</v>
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 28</v>
       </c>
       <c r="B17" s="5">
         <v>45526.362384259257</v>
@@ -3650,21 +3586,20 @@
         <v>122</v>
       </c>
       <c r="D17" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday27</v>
+        <f t="shared" si="1"/>
+        <v>gpxday28</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>225</v>
+        <v>176</v>
       </c>
       <c r="G17" t="s">
-        <v>271</v>
+        <v>222</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="1" t="s">
@@ -3748,8 +3683,9 @@
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>180</v>
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 27</v>
       </c>
       <c r="B18" s="5">
         <v>45525.413229166668</v>
@@ -3758,18 +3694,17 @@
         <v>122</v>
       </c>
       <c r="D18" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday26</v>
+        <f t="shared" si="1"/>
+        <v>gpxday27</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>226</v>
+        <v>177</v>
       </c>
       <c r="G18" t="s">
-        <v>272</v>
+        <v>223</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -3854,8 +3789,9 @@
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>181</v>
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 26</v>
       </c>
       <c r="B19" s="5">
         <v>45524.418935185182</v>
@@ -3864,18 +3800,17 @@
         <v>122</v>
       </c>
       <c r="D19" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday25</v>
+        <f t="shared" si="1"/>
+        <v>gpxday26</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>227</v>
+        <v>178</v>
       </c>
       <c r="G19" t="s">
-        <v>273</v>
+        <v>224</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -3960,8 +3895,9 @@
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>182</v>
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 25</v>
       </c>
       <c r="B20" s="5">
         <v>45523.405543981484</v>
@@ -3970,21 +3906,24 @@
         <v>122</v>
       </c>
       <c r="D20" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday24</v>
+        <f t="shared" si="1"/>
+        <v>gpxday25</v>
       </c>
       <c r="E20">
-        <f t="shared" si="1"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>228</v>
+        <v>179</v>
       </c>
       <c r="G20" t="s">
+        <v>225</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
       <c r="J20" s="1" t="s">
         <v>48</v>
       </c>
@@ -4066,8 +4005,9 @@
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>183</v>
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 24</v>
       </c>
       <c r="B21" s="5">
         <v>45522.654398148145</v>
@@ -4076,21 +4016,24 @@
         <v>121</v>
       </c>
       <c r="D21" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday23</v>
+        <f t="shared" si="1"/>
+        <v>gpxday24</v>
       </c>
       <c r="E21">
-        <f t="shared" si="1"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>229</v>
+        <v>180</v>
       </c>
       <c r="G21" t="s">
-        <v>275</v>
-      </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+        <v>226</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="I21" t="s">
+        <v>267</v>
+      </c>
       <c r="J21" s="1" t="s">
         <v>50</v>
       </c>
@@ -4172,8 +4115,9 @@
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>184</v>
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 23</v>
       </c>
       <c r="B22" s="5">
         <v>45521.442673611113</v>
@@ -4182,21 +4126,24 @@
         <v>122</v>
       </c>
       <c r="D22" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday22</v>
+        <f t="shared" si="1"/>
+        <v>gpxday23</v>
       </c>
       <c r="E22">
-        <f t="shared" si="1"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>230</v>
+        <v>181</v>
       </c>
       <c r="G22" t="s">
-        <v>276</v>
-      </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+        <v>227</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="I22" t="s">
+        <v>267</v>
+      </c>
       <c r="J22" s="1" t="s">
         <v>52</v>
       </c>
@@ -4278,8 +4225,9 @@
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>185</v>
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 22</v>
       </c>
       <c r="B23" s="5">
         <v>45520.589930555558</v>
@@ -4288,21 +4236,24 @@
         <v>122</v>
       </c>
       <c r="D23" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday21</v>
+        <f t="shared" si="1"/>
+        <v>gpxday22</v>
       </c>
       <c r="E23">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>231</v>
+        <v>182</v>
       </c>
       <c r="G23" t="s">
-        <v>277</v>
-      </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+        <v>228</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="I23" t="s">
+        <v>267</v>
+      </c>
       <c r="J23" s="1" t="s">
         <v>54</v>
       </c>
@@ -4384,8 +4335,9 @@
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>186</v>
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 21</v>
       </c>
       <c r="B24" s="5">
         <v>45519.483831018515</v>
@@ -4394,21 +4346,24 @@
         <v>122</v>
       </c>
       <c r="D24" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday20</v>
+        <f t="shared" si="1"/>
+        <v>gpxday21</v>
       </c>
       <c r="E24">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>232</v>
+        <v>183</v>
       </c>
       <c r="G24" t="s">
-        <v>278</v>
-      </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+        <v>229</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="I24" t="s">
+        <v>267</v>
+      </c>
       <c r="J24" s="1" t="s">
         <v>56</v>
       </c>
@@ -4490,8 +4445,9 @@
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>187</v>
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 20</v>
       </c>
       <c r="B25" s="5">
         <v>45518.441921296297</v>
@@ -4500,21 +4456,24 @@
         <v>122</v>
       </c>
       <c r="D25" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday19</v>
+        <f t="shared" si="1"/>
+        <v>gpxday20</v>
       </c>
       <c r="E25">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>233</v>
+        <v>184</v>
       </c>
       <c r="G25" t="s">
-        <v>279</v>
-      </c>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+        <v>230</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="I25" t="s">
+        <v>267</v>
+      </c>
       <c r="J25" s="1" t="s">
         <v>58</v>
       </c>
@@ -4596,8 +4555,9 @@
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>188</v>
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 19</v>
       </c>
       <c r="B26" s="5">
         <v>45517.373657407406</v>
@@ -4606,21 +4566,24 @@
         <v>122</v>
       </c>
       <c r="D26" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday18</v>
+        <f t="shared" si="1"/>
+        <v>gpxday19</v>
       </c>
       <c r="E26">
-        <f t="shared" si="1"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>234</v>
+        <v>185</v>
       </c>
       <c r="G26" t="s">
-        <v>280</v>
-      </c>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
+        <v>231</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="I26" t="s">
+        <v>267</v>
+      </c>
       <c r="J26" s="1" t="s">
         <v>60</v>
       </c>
@@ -4702,8 +4665,9 @@
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>189</v>
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 18</v>
       </c>
       <c r="B27" s="5">
         <v>45516.385358796295</v>
@@ -4712,21 +4676,24 @@
         <v>122</v>
       </c>
       <c r="D27" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday17</v>
+        <f t="shared" si="1"/>
+        <v>gpxday18</v>
       </c>
       <c r="E27">
-        <f t="shared" si="1"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>235</v>
+        <v>186</v>
       </c>
       <c r="G27" t="s">
-        <v>281</v>
-      </c>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
+        <v>232</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>266</v>
+      </c>
       <c r="J27" s="1" t="s">
         <v>62</v>
       </c>
@@ -4808,8 +4775,9 @@
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>190</v>
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 17</v>
       </c>
       <c r="B28" s="5">
         <v>45515.403310185182</v>
@@ -4818,21 +4786,24 @@
         <v>122</v>
       </c>
       <c r="D28" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday16</v>
+        <f t="shared" si="1"/>
+        <v>gpxday17</v>
       </c>
       <c r="E28">
-        <f t="shared" si="1"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>236</v>
+        <v>187</v>
       </c>
       <c r="G28" t="s">
-        <v>282</v>
-      </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
+        <v>233</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="J28" s="1" t="s">
         <v>64</v>
       </c>
@@ -4914,8 +4885,9 @@
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>191</v>
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 16</v>
       </c>
       <c r="B29" s="5">
         <v>45514.453009259261</v>
@@ -4924,21 +4896,24 @@
         <v>122</v>
       </c>
       <c r="D29" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday15</v>
+        <f t="shared" si="1"/>
+        <v>gpxday16</v>
       </c>
       <c r="E29">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>237</v>
+        <v>188</v>
       </c>
       <c r="G29" t="s">
-        <v>283</v>
-      </c>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
+        <v>234</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="J29" s="1" t="s">
         <v>66</v>
       </c>
@@ -5020,8 +4995,9 @@
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>192</v>
+      <c r="A30" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 15</v>
       </c>
       <c r="B30" s="5">
         <v>45513.450868055559</v>
@@ -5030,21 +5006,24 @@
         <v>122</v>
       </c>
       <c r="D30" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday14</v>
+        <f t="shared" si="1"/>
+        <v>gpxday15</v>
       </c>
       <c r="E30">
-        <f t="shared" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>238</v>
+        <v>189</v>
       </c>
       <c r="G30" t="s">
-        <v>284</v>
-      </c>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
+        <v>235</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="J30" s="1" t="s">
         <v>68</v>
       </c>
@@ -5126,8 +5105,9 @@
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>193</v>
+      <c r="A31" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 14</v>
       </c>
       <c r="B31" s="5">
         <v>45512.549513888887</v>
@@ -5136,21 +5116,24 @@
         <v>122</v>
       </c>
       <c r="D31" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday13</v>
+        <f t="shared" si="1"/>
+        <v>gpxday14</v>
       </c>
       <c r="E31">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>239</v>
+        <v>190</v>
       </c>
       <c r="G31" t="s">
-        <v>285</v>
-      </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
+        <v>236</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="J31" s="1" t="s">
         <v>70</v>
       </c>
@@ -5232,8 +5215,9 @@
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>194</v>
+      <c r="A32" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 13</v>
       </c>
       <c r="B32" s="5">
         <v>45511</v>
@@ -5242,24 +5226,25 @@
         <v>122</v>
       </c>
       <c r="D32" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday12</v>
+        <f t="shared" si="1"/>
+        <v>gpxday13</v>
       </c>
       <c r="E32">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>240</v>
+        <v>191</v>
       </c>
       <c r="G32" t="s">
-        <v>286</v>
+        <v>237</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="I32" s="5"/>
-      <c r="J32" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="J32" s="19" t="s">
         <v>114</v>
       </c>
       <c r="K32" s="1">
@@ -5340,8 +5325,9 @@
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>195</v>
+      <c r="A33" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 12</v>
       </c>
       <c r="B33" s="5">
         <v>45510.433611111112</v>
@@ -5350,23 +5336,25 @@
         <v>122</v>
       </c>
       <c r="D33" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>gpxday11</v>
+        <f t="shared" si="1"/>
+        <v>gpxday12</v>
       </c>
       <c r="E33">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>241</v>
+        <v>192</v>
       </c>
       <c r="G33" t="s">
-        <v>287</v>
+        <v>238</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="I33" s="5"/>
-      <c r="J33" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="J33" s="19" t="s">
         <v>113</v>
       </c>
       <c r="K33" s="1">
@@ -5447,8 +5435,9 @@
       </c>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>163</v>
+      <c r="A34" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 11</v>
       </c>
       <c r="B34" s="5">
         <v>45509</v>
@@ -5457,18 +5446,23 @@
         <v>112</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>209</v>
+        <v>161</v>
+      </c>
+      <c r="E34">
+        <v>11</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>242</v>
+        <v>193</v>
       </c>
       <c r="G34" t="s">
-        <v>288</v>
+        <v>239</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="I34" s="5"/>
+        <v>135</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="J34" s="1" t="s">
         <v>123</v>
       </c>
@@ -5504,8 +5498,9 @@
       </c>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>196</v>
+      <c r="A35" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 10</v>
       </c>
       <c r="B35" s="5">
         <v>45508.37740740741</v>
@@ -5514,23 +5509,24 @@
         <v>122</v>
       </c>
       <c r="D35" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>gpxday10</v>
       </c>
       <c r="E35">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>243</v>
+        <v>194</v>
       </c>
       <c r="G35" t="s">
-        <v>289</v>
+        <v>240</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="I35" s="5"/>
+        <v>135</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="J35" s="1" t="s">
         <v>74</v>
       </c>
@@ -5612,8 +5608,9 @@
       </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>197</v>
+      <c r="A36" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 9</v>
       </c>
       <c r="B36" s="5">
         <v>45507.421967592592</v>
@@ -5622,21 +5619,24 @@
         <v>122</v>
       </c>
       <c r="D36" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>gpxday9</v>
       </c>
       <c r="E36">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>244</v>
+        <v>195</v>
       </c>
       <c r="G36" t="s">
-        <v>290</v>
-      </c>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
+        <v>241</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="J36" s="1" t="s">
         <v>76</v>
       </c>
@@ -5718,8 +5718,9 @@
       </c>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>198</v>
+      <c r="A37" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 8</v>
       </c>
       <c r="B37" s="5">
         <v>45506.403993055559</v>
@@ -5728,21 +5729,24 @@
         <v>122</v>
       </c>
       <c r="D37" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>gpxday8</v>
       </c>
       <c r="E37">
-        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>245</v>
+        <v>196</v>
       </c>
       <c r="G37" t="s">
-        <v>291</v>
-      </c>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
+        <v>242</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="J37" s="1" t="s">
         <v>78</v>
       </c>
@@ -5824,8 +5828,9 @@
       </c>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>199</v>
+      <c r="A38" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 7</v>
       </c>
       <c r="B38" s="5">
         <v>45505.452870370369</v>
@@ -5834,24 +5839,23 @@
         <v>122</v>
       </c>
       <c r="D38" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>gpxday7</v>
       </c>
       <c r="E38">
-        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>246</v>
+        <v>197</v>
       </c>
       <c r="G38" t="s">
-        <v>292</v>
+        <v>243</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>132</v>
+        <v>254</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>80</v>
@@ -5934,8 +5938,9 @@
       </c>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>200</v>
+      <c r="A39" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 6</v>
       </c>
       <c r="B39" s="5">
         <v>45504.391481481478</v>
@@ -5944,24 +5949,23 @@
         <v>122</v>
       </c>
       <c r="D39" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>gpxday6</v>
       </c>
       <c r="E39">
-        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>247</v>
+        <v>198</v>
       </c>
       <c r="G39" t="s">
-        <v>293</v>
+        <v>244</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>131</v>
+        <v>253</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>82</v>
@@ -6044,8 +6048,9 @@
       </c>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>201</v>
+      <c r="A40" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 5</v>
       </c>
       <c r="B40" s="5">
         <v>45503.407893518517</v>
@@ -6054,24 +6059,23 @@
         <v>122</v>
       </c>
       <c r="D40" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>gpxday5</v>
       </c>
       <c r="E40">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="G40" t="s">
-        <v>294</v>
+        <v>245</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>130</v>
+        <v>256</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>84</v>
@@ -6154,8 +6158,9 @@
       </c>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>202</v>
+      <c r="A41" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 4</v>
       </c>
       <c r="B41" s="5">
         <v>45502.385138888887</v>
@@ -6164,24 +6169,23 @@
         <v>122</v>
       </c>
       <c r="D41" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>gpxday4</v>
       </c>
       <c r="E41">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>249</v>
+        <v>200</v>
       </c>
       <c r="G41" t="s">
-        <v>295</v>
+        <v>246</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>129</v>
+        <v>255</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>86</v>
@@ -6264,8 +6268,9 @@
       </c>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>203</v>
+      <c r="A42" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 3</v>
       </c>
       <c r="B42" s="5">
         <v>45501.56591435185</v>
@@ -6274,24 +6279,23 @@
         <v>122</v>
       </c>
       <c r="D42" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>gpxday3</v>
       </c>
       <c r="E42">
-        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>250</v>
+        <v>201</v>
       </c>
       <c r="G42" t="s">
-        <v>296</v>
+        <v>247</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>128</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>87</v>
@@ -6374,8 +6378,9 @@
       </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>204</v>
+      <c r="A43" t="str">
+        <f t="shared" si="0"/>
+        <v>Day 2</v>
       </c>
       <c r="B43" s="5">
         <v>45500.426550925928</v>
@@ -6384,24 +6389,23 @@
         <v>121</v>
       </c>
       <c r="D43" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>gpxday2</v>
       </c>
       <c r="E43">
-        <f>E44+1</f>
         <v>2</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>213</v>
+        <v>164</v>
       </c>
       <c r="G43" t="s">
-        <v>297</v>
+        <v>248</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>88</v>
@@ -6484,8 +6488,9 @@
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>205</v>
+      <c r="A44" t="str">
+        <f>"Day "&amp;E44</f>
+        <v>Day 1</v>
       </c>
       <c r="B44" s="5">
         <v>45499.423356481479</v>
@@ -6501,16 +6506,16 @@
         <v>1</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>212</v>
+        <v>163</v>
       </c>
       <c r="G44" t="s">
-        <v>298</v>
+        <v>249</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>127</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>90</v>
@@ -6601,7 +6606,7 @@
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="M45" s="1">
         <v>1284068</v>
@@ -6637,7 +6642,7 @@
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="7" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="M46">
         <v>1340966</v>
@@ -6648,38 +6653,50 @@
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.2">
       <c r="H47" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="1" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.2">
       <c r="H48" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I48" s="5"/>
       <c r="J48" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="10:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H49" s="5" t="s">
+        <v>250</v>
+      </c>
       <c r="J49" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="10:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H50" s="5" t="s">
+        <v>260</v>
+      </c>
       <c r="J50" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="10:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H51" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="J51" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="52" spans="10:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H52" s="5" t="s">
+        <v>251</v>
+      </c>
       <c r="J52" s="7" t="s">
         <v>118</v>
       </c>
@@ -6706,7 +6723,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="53" spans="10:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="8:17" x14ac:dyDescent="0.2">
       <c r="J53" s="7" t="s">
         <v>119</v>
       </c>
@@ -6733,9 +6750,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="10:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="8:17" x14ac:dyDescent="0.2">
       <c r="L54" s="10" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="M54" s="10">
         <v>35</v>
@@ -6745,7 +6762,7 @@
         <v>7.5868253968253958</v>
       </c>
       <c r="O54" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="P54" s="11">
         <f>K52/M54</f>
@@ -6756,7 +6773,7 @@
         <v>1475.2857142857142</v>
       </c>
     </row>
-    <row r="55" spans="10:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="8:17" x14ac:dyDescent="0.2">
       <c r="M55">
         <v>37</v>
       </c>
@@ -6765,7 +6782,7 @@
         <v>7.1767267267267272</v>
       </c>
       <c r="O55" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="P55" s="11">
         <f>K53/M55</f>

</xml_diff>

<commit_message>
tuning the tabulator table
</commit_message>
<xml_diff>
--- a/projects/en/docs/assets/tables/GDMBR.xlsx
+++ b/projects/en/docs/assets/tables/GDMBR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gravel/Private/f3/projects/en/docs/assets/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBCB0F4-DCE3-1D48-B48F-39938FF469B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F8DCCB-4FC5-474A-BD86-95D59310B59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6680" yWindow="3980" windowWidth="33860" windowHeight="23260" xr2:uid="{3D076BE0-CA79-3448-855F-AD0FA0DCE9D7}"/>
+    <workbookView xWindow="1200" yWindow="3880" windowWidth="33860" windowHeight="23260" xr2:uid="{3D076BE0-CA79-3448-855F-AD0FA0DCE9D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="281">
   <si>
     <t>When</t>
   </si>
@@ -502,35 +502,7 @@
     <t>1750.41 km so far ; more info + photos : https://siroccomeister.github.io/f3/blog/</t>
   </si>
   <si>
-    <r>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF032E"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>My Great Divide - Day 15 - from Dillon to Dubois</t>
-    </r>
-  </si>
-  <si>
     <t>1515.08 km so far ; more info + photos : https://siroccomeister.github.io/f3/blog/</t>
-  </si>
-  <si>
-    <r>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF032E"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>My Great Divide - Day 16 - from Dillon to Dillon</t>
-    </r>
   </si>
   <si>
     <t>1607.55 km so far ; more info + photos : https://siroccomeister.github.io/f3/blog/</t>
@@ -1322,6 +1294,18 @@
     <t>no blog…</t>
   </si>
   <si>
+    <t>Steamboat Springs</t>
+  </si>
+  <si>
+    <t>Silverthorne, Breckenridge, Boreas Pass, Hartsel</t>
+  </si>
+  <si>
+    <t>Passing Kremmling</t>
+  </si>
+  <si>
+    <t>Leaving Salida</t>
+  </si>
+  <si>
     <r>
       <t> </t>
     </r>
@@ -1341,7 +1325,7 @@
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
-      <t>from Helena West Side to Butte</t>
+      <t>from Helena Valley Northwest to Helena West Side</t>
     </r>
   </si>
   <si>
@@ -1364,20 +1348,36 @@
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
-      <t>from Helena Valley Northwest to Helena West Side</t>
-    </r>
-  </si>
-  <si>
-    <t>Steamboat Springs</t>
-  </si>
-  <si>
-    <t>Silverthorne, Breckenridge, Boreas Pass, Hartsel</t>
-  </si>
-  <si>
-    <t>Passing Kremmling</t>
-  </si>
-  <si>
-    <t>Leaving Salida</t>
+      <t>from Helena West Side to Butte</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF032E"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>My Great Divide - Day 15 - from Dillon to Dillon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF032E"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>My Great Divide - Day 16 - from Dillon to Dubois</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1481,7 +1481,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1512,7 +1512,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1851,7 +1850,7 @@
   <dimension ref="A1:AI56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1859,7 +1858,7 @@
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="8.1640625" customWidth="1"/>
     <col min="7" max="7" width="39.6640625" bestFit="1" customWidth="1"/>
@@ -1884,1733 +1883,1715 @@
   <sheetData>
     <row r="1" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="N1" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="O1" s="15" t="s">
         <v>93</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="P1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="Q1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="S1" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="T1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="U1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="V1" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="W1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="X1" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="Y1" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="Z1" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="Y1" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z1" s="14" t="s">
-        <v>105</v>
       </c>
       <c r="AA1" s="14" t="s">
         <v>3</v>
       </c>
       <c r="AB1" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AC1" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AD1" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AE1" s="14" t="s">
         <v>4</v>
       </c>
       <c r="AF1" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AG1" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AH1" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AI1" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="5">
+        <v>109</v>
+      </c>
+      <c r="B2" s="21">
         <v>45545</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>109</v>
+      </c>
+      <c r="D2" s="5" t="str">
+        <f t="shared" ref="D2:D16" si="0">"gpxday"&amp;E2</f>
+        <v>gpxday42.5</v>
       </c>
       <c r="E2">
-        <v>43</v>
+        <v>42.5</v>
       </c>
       <c r="F2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G2" t="s">
         <v>199</v>
       </c>
-      <c r="G2" t="s">
-        <v>201</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>140</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="K2" s="1">
-        <v>72.33</v>
-      </c>
-      <c r="L2" s="1">
-        <v>165</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0.14210648148148147</v>
-      </c>
-      <c r="N2" s="6">
-        <v>0.13082175925925926</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0.27126157407407409</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>23</v>
-      </c>
-      <c r="R2" s="1">
-        <v>35.4</v>
-      </c>
-      <c r="S2" s="3">
-        <v>0.10833333333333334</v>
-      </c>
-      <c r="T2" s="3">
-        <v>0.11805555555555555</v>
-      </c>
-      <c r="U2" s="3">
-        <v>7.0833333333333331E-2</v>
-      </c>
-      <c r="V2" s="3">
-        <v>1.1111111111111112E-2</v>
-      </c>
-      <c r="W2" s="3">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="X2" s="1">
-        <v>129</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>1440</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>1316</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>92.1</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>53</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>23</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>2013</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>1454</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>67.459999999999994</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI2" s="18">
-        <f t="shared" ref="AI2:AI43" si="0">AI3+K2</f>
-        <v>4581.2200000000012</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>"Day "&amp;E3</f>
+        <f t="shared" ref="A3:A16" si="1">"Day "&amp;E3</f>
         <v>Day 42</v>
       </c>
       <c r="B3" s="5">
         <v>45541.271261574075</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D3" s="5" t="str">
-        <f>"gpxday"&amp;E3</f>
+        <f t="shared" si="0"/>
         <v>gpxday42</v>
       </c>
       <c r="E3">
         <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="J3" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="J3" s="20" t="s">
-        <v>273</v>
-      </c>
       <c r="K3" s="1">
-        <v>188.45</v>
+        <v>72.33</v>
       </c>
       <c r="L3" s="1">
-        <v>1592</v>
+        <v>165</v>
       </c>
       <c r="M3" s="2">
-        <v>0.54045138888888888</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0.41767361111111112</v>
+        <v>0.14210648148148147</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0.13082175925925926</v>
       </c>
       <c r="O3" s="2">
-        <v>0.3313888888888889</v>
+        <v>0.27126157407407409</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q3" s="1">
-        <v>18.8</v>
+        <v>23</v>
       </c>
       <c r="R3" s="1">
-        <v>59.6</v>
+        <v>35.4</v>
       </c>
       <c r="S3" s="3">
-        <v>0.13333333333333333</v>
+        <v>0.10833333333333334</v>
       </c>
       <c r="T3" s="3">
-        <v>0.17222222222222222</v>
+        <v>0.11805555555555555</v>
       </c>
       <c r="U3" s="3">
-        <v>4.1666666666666664E-2</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="V3" s="3">
-        <v>1.3194444444444444E-2</v>
+        <v>1.1111111111111112E-2</v>
       </c>
       <c r="W3" s="3">
-        <v>4.1666666666666666E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="X3" s="1">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="Y3" s="1">
-        <v>2290</v>
+        <v>1440</v>
       </c>
       <c r="Z3" s="1">
-        <v>1344</v>
+        <v>1316</v>
       </c>
       <c r="AA3" s="1">
-        <v>77.3</v>
+        <v>92.1</v>
       </c>
       <c r="AB3" s="1">
-        <v>8.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AC3" s="1">
-        <v>159</v>
+        <v>53</v>
       </c>
       <c r="AD3" s="1">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="AE3" s="1">
-        <v>5682</v>
+        <v>2013</v>
       </c>
       <c r="AF3" s="1">
-        <v>3699</v>
+        <v>1454</v>
       </c>
       <c r="AG3" s="1">
-        <v>124.86</v>
+        <v>67.459999999999994</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="AI3" s="18">
-        <f t="shared" si="0"/>
-        <v>4508.8900000000012</v>
+        <f>AI4+K3</f>
+        <v>4581.2200000000012</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>"Day "&amp;E4</f>
+        <f t="shared" si="1"/>
         <v>Day 41</v>
       </c>
       <c r="B4" s="5">
         <v>45540.331388888888</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D4" s="5" t="str">
-        <f>"gpxday"&amp;E4</f>
+        <f t="shared" si="0"/>
         <v>gpxday41</v>
       </c>
       <c r="E4">
         <v>41</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="1">
-        <v>90.37</v>
+        <v>188.45</v>
       </c>
       <c r="L4" s="1">
-        <v>1578</v>
+        <v>1592</v>
       </c>
       <c r="M4" s="2">
-        <v>0.41324074074074074</v>
+        <v>0.54045138888888888</v>
       </c>
       <c r="N4" s="2">
-        <v>0.22233796296296296</v>
+        <v>0.41767361111111112</v>
       </c>
       <c r="O4" s="2">
-        <v>0.36148148148148146</v>
+        <v>0.3313888888888889</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="Q4" s="1">
-        <v>16.899999999999999</v>
+        <v>18.8</v>
       </c>
       <c r="R4" s="1">
-        <v>59.2</v>
+        <v>59.6</v>
       </c>
       <c r="S4" s="3">
-        <v>0.14791666666666667</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="T4" s="3">
-        <v>0.27430555555555558</v>
+        <v>0.17222222222222222</v>
       </c>
       <c r="U4" s="3">
-        <v>4.2361111111111113E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="V4" s="3">
-        <v>1.4583333333333334E-2</v>
+        <v>1.3194444444444444E-2</v>
       </c>
       <c r="W4" s="3">
         <v>4.1666666666666666E-3</v>
       </c>
       <c r="X4" s="1">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="Y4" s="1">
-        <v>2434</v>
+        <v>2290</v>
       </c>
       <c r="Z4" s="1">
-        <v>1828</v>
+        <v>1344</v>
       </c>
       <c r="AA4" s="1">
-        <v>53.8</v>
+        <v>77.3</v>
       </c>
       <c r="AB4" s="1">
-        <v>17.5</v>
+        <v>8.4</v>
       </c>
       <c r="AC4" s="1">
-        <v>296</v>
+        <v>159</v>
       </c>
       <c r="AD4" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AE4" s="1">
-        <v>3425</v>
+        <v>5682</v>
       </c>
       <c r="AF4" s="1">
-        <v>2209</v>
+        <v>3699</v>
       </c>
       <c r="AG4" s="1">
-        <v>44.35</v>
+        <v>124.86</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AI4" s="18">
-        <f t="shared" si="0"/>
-        <v>4320.4400000000014</v>
+        <f>AI5+K4</f>
+        <v>4508.8900000000012</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>"Day "&amp;E5</f>
+        <f t="shared" si="1"/>
         <v>Day 40</v>
       </c>
       <c r="B5" s="5">
         <v>45539.361481481479</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D5" s="5" t="str">
-        <f>"gpxday"&amp;E5</f>
+        <f t="shared" si="0"/>
         <v>gpxday40</v>
       </c>
       <c r="E5">
-        <f>E4-1</f>
+        <f t="shared" ref="E5:E17" si="2">E4-1</f>
         <v>40</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K5" s="1">
-        <v>156.62</v>
+        <v>90.37</v>
       </c>
       <c r="L5" s="1">
-        <v>1241</v>
+        <v>1578</v>
       </c>
       <c r="M5" s="2">
-        <v>0.40164351851851854</v>
+        <v>0.41324074074074074</v>
       </c>
       <c r="N5" s="2">
-        <v>0.32800925925925928</v>
+        <v>0.22233796296296296</v>
       </c>
       <c r="O5" s="2">
-        <v>0.31719907407407405</v>
+        <v>0.36148148148148146</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="Q5" s="1">
-        <v>19.899999999999999</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="R5" s="1">
-        <v>46.6</v>
+        <v>59.2</v>
       </c>
       <c r="S5" s="3">
-        <v>0.12569444444444444</v>
+        <v>0.14791666666666667</v>
       </c>
       <c r="T5" s="3">
-        <v>0.15416666666666667</v>
+        <v>0.27430555555555558</v>
       </c>
       <c r="U5" s="3">
-        <v>5.347222222222222E-2</v>
+        <v>4.2361111111111113E-2</v>
       </c>
       <c r="V5" s="3">
-        <v>1.2500000000000001E-2</v>
+        <v>1.4583333333333334E-2</v>
       </c>
       <c r="W5" s="3">
-        <v>5.5555555555555558E-3</v>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="X5" s="1">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="Y5" s="1">
-        <v>2529</v>
+        <v>2434</v>
       </c>
       <c r="Z5" s="1">
-        <v>2052</v>
+        <v>1828</v>
       </c>
       <c r="AA5" s="1">
-        <v>81.7</v>
+        <v>53.8</v>
       </c>
       <c r="AB5" s="1">
-        <v>7.9</v>
+        <v>17.5</v>
       </c>
       <c r="AC5" s="1">
-        <v>158</v>
+        <v>296</v>
       </c>
       <c r="AD5" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="AE5" s="1">
-        <v>4736</v>
+        <v>3425</v>
       </c>
       <c r="AF5" s="1">
-        <v>3054</v>
+        <v>2209</v>
       </c>
       <c r="AG5" s="1">
-        <v>96.3</v>
-      </c>
-      <c r="AH5" s="12" t="s">
-        <v>17</v>
+        <v>44.35</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="AI5" s="18">
-        <f t="shared" si="0"/>
-        <v>4230.0700000000015</v>
+        <f>AI6+K5</f>
+        <v>4320.4400000000014</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>"Day "&amp;E6</f>
+        <f t="shared" si="1"/>
         <v>Day 39</v>
       </c>
       <c r="B6" s="5">
         <v>45538.317199074074</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D6" s="5" t="str">
-        <f>"gpxday"&amp;E6</f>
+        <f t="shared" si="0"/>
         <v>gpxday39</v>
       </c>
       <c r="E6">
-        <f>E5-1</f>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K6" s="1">
-        <v>115.39</v>
+        <v>156.62</v>
       </c>
       <c r="L6" s="1">
-        <v>824</v>
+        <v>1241</v>
       </c>
       <c r="M6" s="2">
-        <v>0.4037384259259259</v>
+        <v>0.40164351851851854</v>
       </c>
       <c r="N6" s="2">
-        <v>0.2633564814814815</v>
+        <v>0.32800925925925928</v>
       </c>
       <c r="O6" s="2">
-        <v>0.33015046296296297</v>
+        <v>0.31719907407407405</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="Q6" s="1">
-        <v>18.3</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="R6" s="1">
-        <v>45.7</v>
+        <v>46.6</v>
       </c>
       <c r="S6" s="3">
-        <v>0.13680555555555557</v>
+        <v>0.12569444444444444</v>
       </c>
       <c r="T6" s="3">
-        <v>0.20972222222222223</v>
+        <v>0.15416666666666667</v>
       </c>
       <c r="U6" s="3">
-        <v>5.486111111111111E-2</v>
+        <v>5.347222222222222E-2</v>
       </c>
       <c r="V6" s="3">
-        <v>1.3888888888888888E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="W6" s="3">
         <v>5.5555555555555558E-3</v>
       </c>
       <c r="X6" s="1">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="Y6" s="1">
-        <v>2511</v>
+        <v>2529</v>
       </c>
       <c r="Z6" s="1">
-        <v>2157</v>
+        <v>2052</v>
       </c>
       <c r="AA6" s="1">
-        <v>65.2</v>
+        <v>81.7</v>
       </c>
       <c r="AB6" s="1">
-        <v>7.1</v>
+        <v>7.9</v>
       </c>
       <c r="AC6" s="1">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="AD6" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AE6" s="1">
-        <v>3327</v>
+        <v>4736</v>
       </c>
       <c r="AF6" s="1">
-        <v>2263</v>
+        <v>3054</v>
       </c>
       <c r="AG6" s="1">
-        <v>82.56</v>
+        <v>96.3</v>
       </c>
       <c r="AH6" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI6" s="18">
-        <f t="shared" si="0"/>
-        <v>4073.4500000000012</v>
+        <f>AI7+K6</f>
+        <v>4230.0700000000015</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f>"Day "&amp;E7</f>
+        <f t="shared" si="1"/>
         <v>Day 38</v>
       </c>
       <c r="B7" s="5">
         <v>45537.330150462964</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D7" s="5" t="str">
-        <f>"gpxday"&amp;E7</f>
+        <f t="shared" si="0"/>
         <v>gpxday38</v>
       </c>
       <c r="E7">
-        <f>E6-1</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K7" s="1">
-        <v>97.95</v>
+        <v>115.39</v>
       </c>
       <c r="L7" s="1">
-        <v>1363</v>
+        <v>824</v>
       </c>
       <c r="M7" s="2">
-        <v>0.4614699074074074</v>
+        <v>0.4037384259259259</v>
       </c>
       <c r="N7" s="2">
-        <v>0.27523148148148147</v>
+        <v>0.2633564814814815</v>
       </c>
       <c r="O7" s="2">
-        <v>0.35292824074074075</v>
+        <v>0.33015046296296297</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="Q7" s="1">
-        <v>14.8</v>
+        <v>18.3</v>
       </c>
       <c r="R7" s="1">
-        <v>63.3</v>
+        <v>45.7</v>
       </c>
       <c r="S7" s="3">
-        <v>0.16875000000000001</v>
+        <v>0.13680555555555557</v>
       </c>
       <c r="T7" s="3">
-        <v>0.28263888888888888</v>
+        <v>0.20972222222222223</v>
       </c>
       <c r="U7" s="3">
-        <v>3.9583333333333331E-2</v>
+        <v>5.486111111111111E-2</v>
       </c>
       <c r="V7" s="3">
-        <v>1.6666666666666666E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="W7" s="3">
-        <v>4.1666666666666666E-3</v>
+        <v>5.5555555555555558E-3</v>
       </c>
       <c r="X7" s="1">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="Y7" s="1">
-        <v>2766</v>
+        <v>2511</v>
       </c>
       <c r="Z7" s="1">
-        <v>1961</v>
+        <v>2157</v>
       </c>
       <c r="AA7" s="1">
-        <v>59.6</v>
+        <v>65.2</v>
       </c>
       <c r="AB7" s="1">
-        <v>13.9</v>
+        <v>7.1</v>
       </c>
       <c r="AC7" s="1">
-        <v>206</v>
+        <v>130</v>
       </c>
       <c r="AD7" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AE7" s="1">
-        <v>3136</v>
+        <v>3327</v>
       </c>
       <c r="AF7" s="1">
-        <v>2287</v>
+        <v>2263</v>
       </c>
       <c r="AG7" s="1">
-        <v>67.02</v>
+        <v>82.56</v>
       </c>
       <c r="AH7" s="12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="AI7" s="18">
-        <f t="shared" si="0"/>
-        <v>3958.0600000000013</v>
+        <f>AI8+K7</f>
+        <v>4073.4500000000012</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f>"Day "&amp;E8</f>
+        <f t="shared" si="1"/>
         <v>Day 37</v>
       </c>
       <c r="B8" s="5">
         <v>45536.35292824074</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D8" s="5" t="str">
-        <f>"gpxday"&amp;E8</f>
+        <f t="shared" si="0"/>
         <v>gpxday37</v>
       </c>
       <c r="E8">
-        <f>E7-1</f>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K8" s="1">
-        <v>124.86</v>
+        <v>97.95</v>
       </c>
       <c r="L8" s="1">
-        <v>1140</v>
+        <v>1363</v>
       </c>
       <c r="M8" s="2">
-        <v>0.38868055555555553</v>
+        <v>0.4614699074074074</v>
       </c>
       <c r="N8" s="2">
-        <v>0.30054398148148148</v>
+        <v>0.27523148148148147</v>
       </c>
       <c r="O8" s="2">
-        <v>0.43765046296296295</v>
+        <v>0.35292824074074075</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="Q8" s="1">
-        <v>17.3</v>
+        <v>14.8</v>
       </c>
       <c r="R8" s="1">
-        <v>54.6</v>
+        <v>63.3</v>
       </c>
       <c r="S8" s="3">
-        <v>0.14444444444444443</v>
+        <v>0.16875000000000001</v>
       </c>
       <c r="T8" s="3">
-        <v>0.18680555555555556</v>
+        <v>0.28263888888888888</v>
       </c>
       <c r="U8" s="3">
-        <v>4.583333333333333E-2</v>
+        <v>3.9583333333333331E-2</v>
       </c>
       <c r="V8" s="3">
-        <v>1.4583333333333334E-2</v>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="W8" s="3">
-        <v>4.8611111111111112E-3</v>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="X8" s="1">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Y8" s="1">
-        <v>2108</v>
+        <v>2766</v>
       </c>
       <c r="Z8" s="1">
-        <v>1812</v>
+        <v>1961</v>
       </c>
       <c r="AA8" s="1">
-        <v>77.3</v>
+        <v>59.6</v>
       </c>
       <c r="AB8" s="1">
-        <v>9.1</v>
+        <v>13.9</v>
       </c>
       <c r="AC8" s="1">
-        <v>158</v>
+        <v>206</v>
       </c>
       <c r="AD8" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="AE8" s="1">
-        <v>3772</v>
+        <v>3136</v>
       </c>
       <c r="AF8" s="1">
-        <v>2573</v>
+        <v>2287</v>
       </c>
       <c r="AG8" s="1">
-        <v>80.63</v>
-      </c>
-      <c r="AH8" s="1" t="s">
-        <v>24</v>
+        <v>67.02</v>
+      </c>
+      <c r="AH8" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="AI8" s="18">
-        <f t="shared" si="0"/>
-        <v>3860.1100000000015</v>
+        <f>AI9+K8</f>
+        <v>3958.0600000000013</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
-        <f>"Day "&amp;E9</f>
+        <f t="shared" si="1"/>
         <v>Day 36</v>
       </c>
       <c r="B9" s="5">
         <v>45535.437650462962</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D9" s="5" t="str">
-        <f>"gpxday"&amp;E9</f>
+        <f t="shared" si="0"/>
         <v>gpxday36</v>
       </c>
       <c r="E9">
-        <f>E8-1</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>144</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K9" s="1">
-        <v>124.91</v>
+        <v>124.86</v>
       </c>
       <c r="L9" s="1">
-        <v>2390</v>
+        <v>1140</v>
       </c>
       <c r="M9" s="2">
-        <v>0.4675347222222222</v>
+        <v>0.38868055555555553</v>
       </c>
       <c r="N9" s="2">
-        <v>0.39351851851851855</v>
+        <v>0.30054398148148148</v>
       </c>
       <c r="O9" s="2">
-        <v>0.28628472222222223</v>
+        <v>0.43765046296296295</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q9" s="1">
-        <v>13.2</v>
+        <v>17.3</v>
       </c>
       <c r="R9" s="1">
-        <v>66.900000000000006</v>
+        <v>54.6</v>
       </c>
       <c r="S9" s="3">
-        <v>0.18888888888888888</v>
+        <v>0.14444444444444443</v>
       </c>
       <c r="T9" s="3">
-        <v>0.22430555555555556</v>
+        <v>0.18680555555555556</v>
       </c>
       <c r="U9" s="3">
-        <v>3.7499999999999999E-2</v>
+        <v>4.583333333333333E-2</v>
       </c>
       <c r="V9" s="3">
-        <v>1.8749999999999999E-2</v>
+        <v>1.4583333333333334E-2</v>
       </c>
       <c r="W9" s="3">
-        <v>3.472222222222222E-3</v>
+        <v>4.8611111111111112E-3</v>
       </c>
       <c r="X9" s="1">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="Y9" s="1">
-        <v>3146</v>
+        <v>2108</v>
       </c>
       <c r="Z9" s="1">
-        <v>1823</v>
+        <v>1812</v>
       </c>
       <c r="AA9" s="1">
-        <v>84.2</v>
+        <v>77.3</v>
       </c>
       <c r="AB9" s="1">
-        <v>19.100000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="AC9" s="1">
-        <v>253</v>
+        <v>158</v>
       </c>
       <c r="AD9" s="1">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="AE9" s="1">
-        <v>3100</v>
+        <v>3772</v>
       </c>
       <c r="AF9" s="1">
-        <v>3145</v>
+        <v>2573</v>
       </c>
       <c r="AG9" s="1">
-        <v>61.68</v>
+        <v>80.63</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI9" s="18">
-        <f t="shared" si="0"/>
-        <v>3735.2500000000014</v>
+        <f>AI10+K9</f>
+        <v>3860.1100000000015</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
-        <f>"Day "&amp;E10</f>
+        <f t="shared" si="1"/>
         <v>Day 35</v>
       </c>
       <c r="B10" s="5">
         <v>45534.28628472222</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D10" s="5" t="str">
-        <f>"gpxday"&amp;E10</f>
+        <f t="shared" si="0"/>
         <v>gpxday35</v>
       </c>
       <c r="E10">
-        <f>E9-1</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K10" s="1">
-        <v>88</v>
+        <v>124.91</v>
       </c>
       <c r="L10" s="1">
-        <v>808</v>
+        <v>2390</v>
       </c>
       <c r="M10" s="2">
-        <v>0.25471064814814814</v>
+        <v>0.4675347222222222</v>
       </c>
       <c r="N10" s="2">
-        <v>0.21104166666666666</v>
+        <v>0.39351851851851855</v>
       </c>
       <c r="O10" s="2">
-        <v>0.35076388888888888</v>
+        <v>0.28628472222222223</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q10" s="1">
-        <v>17.399999999999999</v>
+        <v>13.2</v>
       </c>
       <c r="R10" s="1">
-        <v>61.6</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="S10" s="3">
-        <v>0.14374999999999999</v>
+        <v>0.18888888888888888</v>
       </c>
       <c r="T10" s="3">
-        <v>0.1736111111111111</v>
+        <v>0.22430555555555556</v>
       </c>
       <c r="U10" s="3">
-        <v>4.027777777777778E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="V10" s="3">
-        <v>1.4583333333333334E-2</v>
+        <v>1.8749999999999999E-2</v>
       </c>
       <c r="W10" s="3">
-        <v>4.1666666666666666E-3</v>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="X10" s="1">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="Y10" s="1">
-        <v>3056</v>
+        <v>3146</v>
       </c>
       <c r="Z10" s="1">
-        <v>1801</v>
+        <v>1823</v>
       </c>
       <c r="AA10" s="1">
-        <v>82.9</v>
+        <v>84.2</v>
       </c>
       <c r="AB10" s="1">
-        <v>9.1999999999999993</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="AC10" s="1">
-        <v>160</v>
+        <v>253</v>
       </c>
       <c r="AD10" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="AE10" s="1">
-        <v>2763</v>
+        <v>3100</v>
       </c>
       <c r="AF10" s="1">
-        <v>1509</v>
+        <v>3145</v>
       </c>
       <c r="AG10" s="1">
-        <v>55.11</v>
+        <v>61.68</v>
       </c>
       <c r="AH10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="AI10" s="18">
-        <f t="shared" si="0"/>
-        <v>3610.3400000000015</v>
+        <f>AI11+K10</f>
+        <v>3735.2500000000014</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
-        <f>"Day "&amp;E11</f>
+        <f t="shared" si="1"/>
         <v>Day 34</v>
       </c>
       <c r="B11" s="5">
         <v>45533.350763888891</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D11" s="5" t="str">
-        <f>"gpxday"&amp;E11</f>
+        <f t="shared" si="0"/>
         <v>gpxday34</v>
       </c>
       <c r="E11">
-        <f>E10-1</f>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G11" t="s">
-        <v>209</v>
-      </c>
-      <c r="H11" s="5"/>
+        <v>207</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>145</v>
+      </c>
       <c r="I11" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K11" s="1">
-        <v>77.09</v>
+        <v>88</v>
       </c>
       <c r="L11" s="1">
-        <v>1280</v>
+        <v>808</v>
       </c>
       <c r="M11" s="2">
-        <v>0.43944444444444447</v>
+        <v>0.25471064814814814</v>
       </c>
       <c r="N11" s="2">
-        <v>0.2775347222222222</v>
+        <v>0.21104166666666666</v>
       </c>
       <c r="O11" s="2">
-        <v>0.41880787037037037</v>
+        <v>0.35076388888888888</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="Q11" s="1">
-        <v>11.6</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="R11" s="1">
-        <v>48.4</v>
+        <v>61.6</v>
       </c>
       <c r="S11" s="3">
-        <v>0.21597222222222223</v>
+        <v>0.14374999999999999</v>
       </c>
       <c r="T11" s="3">
-        <v>0.34236111111111112</v>
+        <v>0.1736111111111111</v>
       </c>
       <c r="U11" s="3">
-        <v>5.1388888888888887E-2</v>
+        <v>4.027777777777778E-2</v>
       </c>
       <c r="V11" s="3">
-        <v>2.1527777777777778E-2</v>
+        <v>1.4583333333333334E-2</v>
       </c>
       <c r="W11" s="3">
-        <v>4.8611111111111112E-3</v>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="X11" s="1">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="Y11" s="1">
-        <v>3348</v>
+        <v>3056</v>
       </c>
       <c r="Z11" s="1">
-        <v>2676</v>
+        <v>1801</v>
       </c>
       <c r="AA11" s="1">
-        <v>63.2</v>
+        <v>82.9</v>
       </c>
       <c r="AB11" s="1">
-        <v>16.600000000000001</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="AC11" s="1">
-        <v>192</v>
+        <v>160</v>
       </c>
       <c r="AD11" s="1">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="AE11" s="1">
-        <v>2361</v>
+        <v>2763</v>
       </c>
       <c r="AF11" s="1">
-        <v>1793</v>
+        <v>1509</v>
       </c>
       <c r="AG11" s="1">
-        <v>35.61</v>
+        <v>55.11</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AI11" s="18">
-        <f t="shared" si="0"/>
-        <v>3522.3400000000015</v>
+        <f>AI12+K11</f>
+        <v>3610.3400000000015</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
-        <f>"Day "&amp;E12</f>
+        <f t="shared" si="1"/>
         <v>Day 33</v>
       </c>
       <c r="B12" s="5">
         <v>45532.418807870374</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D12" s="5" t="str">
-        <f>"gpxday"&amp;E12</f>
+        <f t="shared" si="0"/>
         <v>gpxday33</v>
       </c>
       <c r="E12">
-        <f>E11-1</f>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G12" t="s">
-        <v>210</v>
+        <v>208</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="K12" s="1">
-        <v>116.96</v>
+        <v>77.09</v>
       </c>
       <c r="L12" s="1">
-        <v>2216</v>
+        <v>1280</v>
       </c>
       <c r="M12" s="2">
-        <v>0.45356481481481481</v>
+        <v>0.43944444444444447</v>
       </c>
       <c r="N12" s="2">
-        <v>0.36295138888888889</v>
+        <v>0.2775347222222222</v>
       </c>
       <c r="O12" s="2">
-        <v>0.3722685185185185</v>
+        <v>0.41880787037037037</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="Q12" s="1">
-        <v>13.4</v>
+        <v>11.6</v>
       </c>
       <c r="R12" s="1">
-        <v>49.8</v>
+        <v>48.4</v>
       </c>
       <c r="S12" s="3">
-        <v>0.18611111111111112</v>
+        <v>0.21597222222222223</v>
       </c>
       <c r="T12" s="3">
-        <v>0.2326388888888889</v>
+        <v>0.34236111111111112</v>
       </c>
       <c r="U12" s="3">
-        <v>0.05</v>
+        <v>5.1388888888888887E-2</v>
       </c>
       <c r="V12" s="3">
-        <v>1.8749999999999999E-2</v>
+        <v>2.1527777777777778E-2</v>
       </c>
       <c r="W12" s="3">
         <v>4.8611111111111112E-3</v>
       </c>
       <c r="X12" s="1">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="Y12" s="1">
-        <v>3637</v>
+        <v>3348</v>
       </c>
       <c r="Z12" s="1">
-        <v>2640</v>
+        <v>2676</v>
       </c>
       <c r="AA12" s="1">
-        <v>80</v>
+        <v>63.2</v>
       </c>
       <c r="AB12" s="1">
-        <v>18.899999999999999</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="AC12" s="1">
-        <v>254</v>
+        <v>192</v>
       </c>
       <c r="AD12" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AE12" s="1">
-        <v>3045</v>
+        <v>2361</v>
       </c>
       <c r="AF12" s="1">
-        <v>2896</v>
+        <v>1793</v>
       </c>
       <c r="AG12" s="1">
-        <v>61.93</v>
-      </c>
-      <c r="AH12" s="12" t="s">
-        <v>32</v>
+        <v>35.61</v>
+      </c>
+      <c r="AH12" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="AI12" s="18">
-        <f t="shared" si="0"/>
-        <v>3445.2500000000014</v>
+        <f>AI13+K12</f>
+        <v>3522.3400000000015</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
-        <f>"Day "&amp;E13</f>
+        <f t="shared" si="1"/>
         <v>Day 32</v>
       </c>
       <c r="B13" s="5">
         <v>45531.37226851852</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D13" s="5" t="str">
-        <f>"gpxday"&amp;E13</f>
+        <f t="shared" si="0"/>
         <v>gpxday32</v>
       </c>
       <c r="E13">
-        <f>E12-1</f>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G13" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>31</v>
       </c>
       <c r="K13" s="1">
-        <v>123.03</v>
+        <v>116.96</v>
       </c>
       <c r="L13" s="1">
-        <v>1497</v>
+        <v>2216</v>
       </c>
       <c r="M13" s="2">
-        <v>0.4511574074074074</v>
+        <v>0.45356481481481481</v>
       </c>
       <c r="N13" s="2">
-        <v>0.32935185185185184</v>
+        <v>0.36295138888888889</v>
       </c>
       <c r="O13" s="2">
-        <v>0.37532407407407409</v>
+        <v>0.3722685185185185</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="Q13" s="1">
-        <v>15.6</v>
+        <v>13.4</v>
       </c>
       <c r="R13" s="1">
-        <v>52.9</v>
+        <v>49.8</v>
       </c>
       <c r="S13" s="3">
-        <v>0.16041666666666668</v>
+        <v>0.18611111111111112</v>
       </c>
       <c r="T13" s="3">
-        <v>0.22013888888888888</v>
+        <v>0.2326388888888889</v>
       </c>
       <c r="U13" s="3">
-        <v>4.7222222222222221E-2</v>
+        <v>0.05</v>
       </c>
       <c r="V13" s="3">
-        <v>1.5972222222222221E-2</v>
+        <v>1.8749999999999999E-2</v>
       </c>
       <c r="W13" s="3">
         <v>4.8611111111111112E-3</v>
       </c>
       <c r="X13" s="1">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="Y13" s="1">
-        <v>3103</v>
+        <v>3637</v>
       </c>
       <c r="Z13" s="1">
-        <v>2390</v>
+        <v>2640</v>
       </c>
       <c r="AA13" s="1">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="AB13" s="1">
-        <v>12.2</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="AC13" s="1">
-        <v>189</v>
+        <v>254</v>
       </c>
       <c r="AD13" s="1">
         <v>19</v>
       </c>
       <c r="AE13" s="1">
-        <v>3887</v>
+        <v>3045</v>
       </c>
       <c r="AF13" s="1">
-        <v>2487</v>
+        <v>2896</v>
       </c>
       <c r="AG13" s="1">
-        <v>70.53</v>
+        <v>61.93</v>
       </c>
       <c r="AH13" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AI13" s="18">
-        <f t="shared" si="0"/>
-        <v>3328.2900000000013</v>
+        <f>AI14+K13</f>
+        <v>3445.2500000000014</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
-        <f>"Day "&amp;E14</f>
+        <f t="shared" si="1"/>
         <v>Day 31</v>
       </c>
       <c r="B14" s="5">
         <v>45530.375324074077</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D14" s="5" t="str">
-        <f>"gpxday"&amp;E14</f>
+        <f t="shared" si="0"/>
         <v>gpxday31</v>
       </c>
       <c r="E14">
-        <f>E13-1</f>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="K14" s="1">
-        <v>112.92</v>
+        <v>123.03</v>
       </c>
       <c r="L14" s="1">
-        <v>1206</v>
+        <v>1497</v>
       </c>
       <c r="M14" s="2">
-        <v>0.40105324074074072</v>
+        <v>0.4511574074074074</v>
       </c>
       <c r="N14" s="2">
-        <v>0.28368055555555555</v>
+        <v>0.32935185185185184</v>
       </c>
       <c r="O14" s="2">
-        <v>0.42564814814814816</v>
+        <v>0.37532407407407409</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="Q14" s="1">
-        <v>16.600000000000001</v>
+        <v>15.6</v>
       </c>
       <c r="R14" s="1">
-        <v>57.1</v>
+        <v>52.9</v>
       </c>
       <c r="S14" s="3">
-        <v>0.15069444444444444</v>
+        <v>0.16041666666666668</v>
       </c>
       <c r="T14" s="3">
-        <v>0.21319444444444444</v>
+        <v>0.22013888888888888</v>
       </c>
       <c r="U14" s="3">
-        <v>4.3749999999999997E-2</v>
+        <v>4.7222222222222221E-2</v>
       </c>
       <c r="V14" s="3">
-        <v>1.5277777777777777E-2</v>
+        <v>1.5972222222222221E-2</v>
       </c>
       <c r="W14" s="3">
-        <v>4.1666666666666666E-3</v>
+        <v>4.8611111111111112E-3</v>
       </c>
       <c r="X14" s="1">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="Y14" s="1">
-        <v>3339</v>
+        <v>3103</v>
       </c>
       <c r="Z14" s="1">
-        <v>2486</v>
+        <v>2390</v>
       </c>
       <c r="AA14" s="1">
-        <v>70.7</v>
+        <v>73</v>
       </c>
       <c r="AB14" s="1">
-        <v>10.7</v>
+        <v>12.2</v>
       </c>
       <c r="AC14" s="1">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="AD14" s="1">
         <v>19</v>
       </c>
       <c r="AE14" s="1">
-        <v>3595</v>
+        <v>3887</v>
       </c>
       <c r="AF14" s="1">
-        <v>2296</v>
+        <v>2487</v>
       </c>
       <c r="AG14" s="1">
-        <v>44.14</v>
+        <v>70.53</v>
       </c>
       <c r="AH14" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AI14" s="18">
-        <f t="shared" si="0"/>
-        <v>3205.2600000000011</v>
+        <f>AI15+K14</f>
+        <v>3328.2900000000013</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f>"Day "&amp;E15</f>
+        <f t="shared" si="1"/>
         <v>Day 30</v>
       </c>
       <c r="B15" s="5">
         <v>45529.42564814815</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D15" s="5" t="str">
-        <f>"gpxday"&amp;E15</f>
+        <f t="shared" si="0"/>
         <v>gpxday30</v>
       </c>
       <c r="E15">
-        <f>E14-1</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>35</v>
       </c>
       <c r="K15" s="1">
-        <v>32.67</v>
+        <v>112.92</v>
       </c>
       <c r="L15" s="1">
-        <v>848</v>
+        <v>1206</v>
       </c>
       <c r="M15" s="2">
-        <v>0.13010416666666666</v>
-      </c>
-      <c r="N15" s="6">
-        <v>0.12092592592592592</v>
+        <v>0.40105324074074072</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0.28368055555555555</v>
       </c>
       <c r="O15" s="2">
-        <v>0.70165509259259262</v>
+        <v>0.42564814814814816</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="Q15" s="1">
-        <v>11.3</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="R15" s="1">
-        <v>25.5</v>
+        <v>57.1</v>
       </c>
       <c r="S15" s="3">
-        <v>0.22222222222222221</v>
+        <v>0.15069444444444444</v>
       </c>
       <c r="T15" s="3">
-        <v>0.2388888888888889</v>
+        <v>0.21319444444444444</v>
       </c>
       <c r="U15" s="3">
-        <v>9.7916666666666666E-2</v>
+        <v>4.3749999999999997E-2</v>
       </c>
       <c r="V15" s="3">
-        <v>2.2222222222222223E-2</v>
+        <v>1.5277777777777777E-2</v>
       </c>
       <c r="W15" s="3">
-        <v>9.7222222222222224E-3</v>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="X15" s="1">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="Y15" s="1">
-        <v>2992</v>
+        <v>3339</v>
       </c>
       <c r="Z15" s="1">
-        <v>2150</v>
+        <v>2486</v>
       </c>
       <c r="AA15" s="1">
-        <v>92.9</v>
+        <v>70.7</v>
       </c>
       <c r="AB15" s="1">
-        <v>26</v>
+        <v>10.7</v>
       </c>
       <c r="AC15" s="1">
-        <v>292</v>
+        <v>177</v>
       </c>
       <c r="AD15" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AE15" s="1">
-        <v>1242</v>
+        <v>3595</v>
       </c>
       <c r="AF15" s="1">
-        <v>1111</v>
+        <v>2296</v>
       </c>
       <c r="AG15" s="1">
-        <v>20.12</v>
-      </c>
-      <c r="AH15" s="1" t="s">
-        <v>38</v>
+        <v>44.14</v>
+      </c>
+      <c r="AH15" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="AI15" s="18">
-        <f>AI17+K15</f>
-        <v>3092.3400000000011</v>
+        <f>AI16+K15</f>
+        <v>3205.2600000000011</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>"Day "&amp;E16</f>
+        <f t="shared" si="1"/>
         <v>Day 29</v>
       </c>
       <c r="B16" s="5">
         <v>45528.701655092591</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D16" s="5" t="str">
-        <f>"gpxday"&amp;E16</f>
+        <f t="shared" si="0"/>
         <v>gpxday29</v>
       </c>
       <c r="E16">
-        <f>E15-1</f>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="1"/>
-      <c r="AF16" s="1"/>
-      <c r="AG16" s="1"/>
-      <c r="AH16" s="1"/>
+      <c r="K16" s="1">
+        <v>32.67</v>
+      </c>
+      <c r="L16" s="1">
+        <v>848</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.13010416666666666</v>
+      </c>
+      <c r="N16" s="6">
+        <v>0.12092592592592592</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0.70165509259259262</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>11.3</v>
+      </c>
+      <c r="R16" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="S16" s="3">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="T16" s="3">
+        <v>0.2388888888888889</v>
+      </c>
+      <c r="U16" s="3">
+        <v>9.7916666666666666E-2</v>
+      </c>
+      <c r="V16" s="3">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="W16" s="3">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="X16" s="1">
+        <v>106</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>2992</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>2150</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>92.9</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>292</v>
+      </c>
+      <c r="AD16" s="1">
+        <v>21</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>1242</v>
+      </c>
+      <c r="AF16" s="1">
+        <v>1111</v>
+      </c>
+      <c r="AG16" s="1">
+        <v>20.12</v>
+      </c>
+      <c r="AH16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI16" s="18">
+        <f>AI17+K16</f>
+        <v>3092.3400000000011</v>
+      </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f t="shared" ref="A3:A44" si="1">"Day "&amp;E17</f>
+        <f t="shared" ref="A17:A44" si="3">"Day "&amp;E17</f>
         <v>Day 28</v>
       </c>
       <c r="B17" s="5">
         <v>45527.323622685188</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D17" s="5" t="str">
-        <f t="shared" ref="D3:D44" si="2">"gpxday"&amp;E17</f>
+        <f t="shared" ref="D17:D44" si="4">"gpxday"&amp;E17</f>
         <v>gpxday28</v>
       </c>
       <c r="E17">
-        <f>E16-1</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G17" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>39</v>
@@ -3688,42 +3669,42 @@
         <v>40</v>
       </c>
       <c r="AI17" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AI2:AI43" si="5">AI18+K17</f>
         <v>3059.670000000001</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 27</v>
       </c>
       <c r="B18" s="5">
         <v>45526.362384259257</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D18" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday27</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="E4:E33" si="3">E17-1</f>
+        <f t="shared" ref="E18:E33" si="6">E17-1</f>
         <v>27</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="J18" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>41</v>
       </c>
       <c r="K18" s="1">
@@ -3799,42 +3780,42 @@
         <v>42</v>
       </c>
       <c r="AI18" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2980.190000000001</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 26</v>
       </c>
       <c r="B19" s="5">
         <v>45525.413229166668</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D19" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday26</v>
       </c>
       <c r="E19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="J19" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>43</v>
       </c>
       <c r="K19" s="1">
@@ -3910,40 +3891,40 @@
         <v>44</v>
       </c>
       <c r="AI19" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2826.7600000000011</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 25</v>
       </c>
       <c r="B20" s="5">
         <v>45524.418935185182</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D20" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday25</v>
       </c>
       <c r="E20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G20" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>45</v>
@@ -4021,40 +4002,40 @@
         <v>46</v>
       </c>
       <c r="AI20" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2720.1600000000012</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 24</v>
       </c>
       <c r="B21" s="5">
         <v>45523.405543981484</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D21" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday24</v>
       </c>
       <c r="E21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G21" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>47</v>
@@ -4132,40 +4113,40 @@
         <v>48</v>
       </c>
       <c r="AI21" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2584.7900000000013</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 23</v>
       </c>
       <c r="B22" s="5">
         <v>45522.654398148145</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D22" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday23</v>
       </c>
       <c r="E22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G22" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I22" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>49</v>
@@ -4243,40 +4224,40 @@
         <v>50</v>
       </c>
       <c r="AI22" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2496.4900000000011</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 22</v>
       </c>
       <c r="B23" s="5">
         <v>45521.442673611113</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D23" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday22</v>
       </c>
       <c r="E23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I23" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>51</v>
@@ -4354,40 +4335,40 @@
         <v>52</v>
       </c>
       <c r="AI23" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2448.170000000001</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 21</v>
       </c>
       <c r="B24" s="5">
         <v>45520.589930555558</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D24" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday21</v>
       </c>
       <c r="E24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>53</v>
@@ -4465,40 +4446,40 @@
         <v>54</v>
       </c>
       <c r="AI24" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2271.9300000000007</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 20</v>
       </c>
       <c r="B25" s="5">
         <v>45519.483831018515</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D25" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday20</v>
       </c>
       <c r="E25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G25" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>55</v>
@@ -4576,40 +4557,40 @@
         <v>56</v>
       </c>
       <c r="AI25" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2090.1800000000007</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 19</v>
       </c>
       <c r="B26" s="5">
         <v>45518.441921296297</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D26" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday19</v>
       </c>
       <c r="E26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>57</v>
@@ -4687,40 +4668,40 @@
         <v>58</v>
       </c>
       <c r="AI26" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1983.8400000000006</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 18</v>
       </c>
       <c r="B27" s="5">
         <v>45517.373657407406</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D27" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday18</v>
       </c>
       <c r="E27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G27" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>59</v>
@@ -4798,40 +4779,40 @@
         <v>60</v>
       </c>
       <c r="AI27" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1886.3400000000006</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 17</v>
       </c>
       <c r="B28" s="5">
         <v>45516.385358796295</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D28" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday17</v>
       </c>
       <c r="E28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>61</v>
@@ -4909,43 +4890,43 @@
         <v>62</v>
       </c>
       <c r="AI28" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1750.1900000000005</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 16</v>
       </c>
       <c r="B29" s="5">
         <v>45515.403310185182</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D29" s="21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday16</v>
       </c>
       <c r="E29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G29" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J29" s="22" t="s">
-        <v>63</v>
+        <v>128</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="K29" s="1">
         <v>131.16</v>
@@ -5017,46 +4998,46 @@
         <v>73.59</v>
       </c>
       <c r="AH29" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AI29" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1607.3300000000004</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 15</v>
       </c>
       <c r="B30" s="5">
         <v>45514.453009259261</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D30" s="21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday15</v>
       </c>
       <c r="E30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G30" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J30" s="22" t="s">
-        <v>65</v>
+        <v>128</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="K30" s="1">
         <v>92.47</v>
@@ -5128,46 +5109,46 @@
         <v>76.790000000000006</v>
       </c>
       <c r="AH30" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AI30" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1476.1700000000003</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 14</v>
       </c>
       <c r="B31" s="5">
         <v>45513.450868055559</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D31" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday14</v>
       </c>
       <c r="E31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G31" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K31" s="1">
         <v>77.510000000000005</v>
@@ -5239,46 +5220,46 @@
         <v>54.83</v>
       </c>
       <c r="AH31" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AI31" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1383.7000000000003</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 13</v>
       </c>
       <c r="B32" s="5">
         <v>45512.549513888887</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D32" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday13</v>
       </c>
       <c r="E32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G32" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K32" s="1">
         <v>64.66</v>
@@ -5350,46 +5331,46 @@
         <v>22.42</v>
       </c>
       <c r="AH32" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AI32" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1306.1900000000003</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 12</v>
       </c>
       <c r="B33" s="5">
         <v>45511</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D33" s="21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday12</v>
       </c>
       <c r="E33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G33" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J33" s="22" t="s">
-        <v>275</v>
+        <v>128</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="K33" s="1">
         <v>92.96</v>
@@ -5461,26 +5442,26 @@
         <v>56.11</v>
       </c>
       <c r="AH33" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AI33" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1241.5300000000002</v>
       </c>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 11</v>
       </c>
       <c r="B34" s="5">
         <v>45510.433611111112</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D34" s="21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday11</v>
       </c>
       <c r="E34">
@@ -5488,19 +5469,19 @@
         <v>11</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G34" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J34" s="22" t="s">
-        <v>276</v>
+        <v>128</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>277</v>
       </c>
       <c r="K34" s="1">
         <v>101.98</v>
@@ -5572,35 +5553,41 @@
         <v>42.01</v>
       </c>
       <c r="AH34" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AI34" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1148.5700000000002</v>
       </c>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" s="5">
+        <v>109</v>
+      </c>
+      <c r="B35" s="21">
         <v>45509</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D35" s="5"/>
+        <v>109</v>
+      </c>
+      <c r="D35" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>gpxday10.5</v>
+      </c>
+      <c r="E35">
+        <v>10.5</v>
+      </c>
       <c r="F35" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G35" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -5629,42 +5616,42 @@
       <c r="AG35" s="1"/>
       <c r="AH35" s="1"/>
       <c r="AI35" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1046.5900000000001</v>
       </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 10</v>
       </c>
       <c r="B36" s="5">
         <v>45508.37740740741</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D36" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday10</v>
       </c>
       <c r="E36">
         <v>10</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G36" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K36" s="1">
         <v>112.87</v>
@@ -5736,45 +5723,45 @@
         <v>84.2</v>
       </c>
       <c r="AH36" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AI36" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1046.5900000000001</v>
       </c>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 9</v>
       </c>
       <c r="B37" s="5">
         <v>45507.421967592592</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D37" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday9</v>
       </c>
       <c r="E37">
         <v>9</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G37" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K37" s="1">
         <v>123.26</v>
@@ -5846,45 +5833,45 @@
         <v>73.42</v>
       </c>
       <c r="AH37" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AI37" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>933.72</v>
       </c>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 8</v>
       </c>
       <c r="B38" s="5">
         <v>45506.403993055559</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D38" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday8</v>
       </c>
       <c r="E38">
         <v>8</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G38" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K38" s="1">
         <v>122.51</v>
@@ -5956,45 +5943,45 @@
         <v>81.78</v>
       </c>
       <c r="AH38" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AI38" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>810.46</v>
       </c>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 7</v>
       </c>
       <c r="B39" s="5">
         <v>45505.452870370369</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D39" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday7</v>
       </c>
       <c r="E39">
         <v>7</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G39" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K39" s="1">
         <v>129.69999999999999</v>
@@ -6066,45 +6053,45 @@
         <v>62.43</v>
       </c>
       <c r="AH39" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AI39" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>687.95</v>
       </c>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 6</v>
       </c>
       <c r="B40" s="5">
         <v>45504.391481481478</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D40" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday6</v>
       </c>
       <c r="E40">
         <v>6</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G40" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K40" s="1">
         <v>130.47999999999999</v>
@@ -6176,45 +6163,45 @@
         <v>76.13</v>
       </c>
       <c r="AH40" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AI40" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>558.25</v>
       </c>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 5</v>
       </c>
       <c r="B41" s="5">
         <v>45503.407893518517</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D41" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday5</v>
       </c>
       <c r="E41">
         <v>5</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G41" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K41" s="1">
         <v>84.67</v>
@@ -6286,45 +6273,45 @@
         <v>58.76</v>
       </c>
       <c r="AH41" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AI41" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>427.77000000000004</v>
       </c>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 4</v>
       </c>
       <c r="B42" s="5">
         <v>45502.385138888887</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D42" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday4</v>
       </c>
       <c r="E42">
         <v>4</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G42" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K42" s="1">
         <v>124.79</v>
@@ -6396,45 +6383,45 @@
         <v>99.16</v>
       </c>
       <c r="AH42" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AI42" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>343.1</v>
       </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 3</v>
       </c>
       <c r="B43" s="5">
         <v>45501.56591435185</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D43" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday3</v>
       </c>
       <c r="E43">
         <v>3</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G43" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K43" s="1">
         <v>48.26</v>
@@ -6506,45 +6493,45 @@
         <v>37.42</v>
       </c>
       <c r="AH43" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AI43" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>218.31</v>
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Day 2</v>
       </c>
       <c r="B44" s="5">
         <v>45500.426550925928</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D44" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>gpxday2</v>
       </c>
       <c r="E44">
         <v>2</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G44" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K44" s="1">
         <v>57.81</v>
@@ -6616,7 +6603,7 @@
         <v>34.44</v>
       </c>
       <c r="AH44" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AI44" s="18">
         <f>AI45+K44</f>
@@ -6632,7 +6619,7 @@
         <v>45499.423356481479</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D45" s="5" t="str">
         <f>"gpxday"&amp;E45</f>
@@ -6642,19 +6629,19 @@
         <v>1</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G45" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K45" s="1">
         <v>112.24</v>
@@ -6726,7 +6713,7 @@
         <v>73.87</v>
       </c>
       <c r="AH45" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AI45" s="18">
         <f>K45</f>
@@ -6742,7 +6729,7 @@
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M46" s="1">
         <v>1284068</v>
@@ -6778,7 +6765,7 @@
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M47">
         <v>1340966</v>
@@ -6789,59 +6776,59 @@
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.2">
       <c r="H48" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I48" s="5"/>
       <c r="J48" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="49" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H49" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H50" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H51" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H52" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H53" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K53" s="8">
-        <f>SUM(K2:K43)</f>
+        <f>SUM(K3:K43)</f>
         <v>4411.170000000001</v>
       </c>
       <c r="L53" s="8">
-        <f>SUM(L2:L43)</f>
+        <f>SUM(L3:L43)</f>
         <v>51635</v>
       </c>
       <c r="N53" s="11">
@@ -6856,12 +6843,12 @@
         <v>194.45362679666087</v>
       </c>
       <c r="Q53" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="8:17" x14ac:dyDescent="0.2">
       <c r="J54" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K54" s="9">
         <f>K53+SUM(K44:K45)</f>
@@ -6883,12 +6870,12 @@
         <v>193.49137445033264</v>
       </c>
       <c r="Q54" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="8:17" x14ac:dyDescent="0.2">
       <c r="L55" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M55" s="10">
         <v>35</v>
@@ -6898,7 +6885,7 @@
         <v>7.5868253968253958</v>
       </c>
       <c r="O55" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="P55" s="11">
         <f>K53/M55</f>
@@ -6918,7 +6905,7 @@
         <v>7.1767267267267272</v>
       </c>
       <c r="O56" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="P56" s="11">
         <f>K54/M56</f>

</xml_diff>